<commit_message>
Added transformer with RL+e load and basic plot for transformer currents and voltages for B4
</commit_message>
<xml_diff>
--- a/config/magnetics.xlsx
+++ b/config/magnetics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q634145\PycharmProjects\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6B5E6F-172A-429C-A6C6-87B06EDCC580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350B5CD2-9B29-412B-A8FE-F83987A90951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="5" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -869,7 +869,7 @@
     <t>LD_tra</t>
   </si>
   <si>
-    <t>SC</t>
+    <t>RL</t>
   </si>
 </sst>
 </file>
@@ -1881,17 +1881,17 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7265625" customWidth="1"/>
+    <col min="5" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1923,8 +1923,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1949,7 +1949,7 @@
       <c r="K13" s="74"/>
       <c r="L13" s="75"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>4</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>5</v>
       </c>
@@ -2076,15 +2076,15 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
     <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
         <v>49</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>50</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="34" t="s">
         <v>51</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
         <v>52</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
         <v>53</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>54</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="34" t="s">
         <v>55</v>
       </c>
@@ -2274,13 +2274,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>96</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>93</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>94</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>95</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>85</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>86</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>87</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>88</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>89</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>92</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="27" t="s">
         <v>90</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>91</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>95</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="27" t="s">
         <v>94</v>
       </c>
@@ -2606,19 +2606,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799FBFCB-8244-4B83-8CC9-EBD2890613E5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="63" t="s">
         <v>126</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="64" t="s">
         <v>239</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>243</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>244</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="65" t="s">
         <v>245</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="65" t="s">
         <v>240</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="65" t="s">
         <v>243</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="65" t="s">
         <v>244</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="65" t="s">
         <v>245</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="65" t="s">
         <v>241</v>
       </c>
@@ -2812,13 +2812,13 @@
         <v>107</v>
       </c>
       <c r="E11" s="12">
-        <v>5</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="F11" s="54" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="65" t="s">
         <v>242</v>
       </c>
@@ -2830,13 +2830,13 @@
         <v>108</v>
       </c>
       <c r="E12" s="12">
-        <v>5.0000000000000001E-3</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="F12" s="54" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="65" t="s">
         <v>250</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="65" t="s">
         <v>249</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="65" t="s">
         <v>251</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="66" t="s">
         <v>252</v>
       </c>
@@ -2939,14 +2939,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.26953125" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="73" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
         <v>197</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>198</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>199</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
         <v>200</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
         <v>201</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>202</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
         <v>203</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
         <v>25</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="33" t="s">
         <v>204</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
         <v>253</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="33" t="s">
         <v>205</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>206</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="34" t="s">
         <v>207</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
         <v>208</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="33" t="s">
         <v>209</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="33" t="s">
         <v>210</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
         <v>211</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="33" t="s">
         <v>212</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="33" t="s">
         <v>213</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="34" t="s">
         <v>214</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="32" t="s">
         <v>215</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="33" t="s">
         <v>216</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>217</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="33" t="s">
         <v>219</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
         <v>220</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="33" t="s">
         <v>221</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>222</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="33" t="s">
         <v>218</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="33" t="s">
         <v>223</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="34" t="s">
         <v>224</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
         <v>152</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="34" t="s">
         <v>49</v>
       </c>
@@ -3660,19 +3660,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD1FA08-9341-462A-B6C2-81B791DE91E0}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="67" t="s">
         <v>261</v>
       </c>
@@ -3711,6 +3711,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{BBA0E1F0-D60B-4F51-8DC8-2DB1107D8149}">
+      <formula1>"NT, OC, SC, RL"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"BMW Group Condensed"&amp;12&amp;KC00000 CONFIDENTIAL</oddFooter>

</xml_diff>

<commit_message>
Added transformer load for B2 and improved plotting
</commit_message>
<xml_diff>
--- a/config/magnetics.xlsx
+++ b/config/magnetics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q634145\PycharmProjects\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350B5CD2-9B29-412B-A8FE-F83987A90951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91CF23F-F82B-4037-8618-D3B85F94CD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
@@ -1881,17 +1881,17 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7265625" customWidth="1"/>
-    <col min="5" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1923,8 +1923,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1949,7 +1949,7 @@
       <c r="K13" s="74"/>
       <c r="L13" s="75"/>
     </row>
-    <row r="14" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>4</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>5</v>
       </c>
@@ -2076,15 +2076,15 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>49</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>50</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>51</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>52</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>53</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>54</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>55</v>
       </c>
@@ -2274,13 +2274,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>96</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>93</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>94</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>95</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>85</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>86</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>87</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>88</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>89</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>92</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>90</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>91</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>95</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>94</v>
       </c>
@@ -2607,18 +2607,18 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="63" t="s">
         <v>126</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>239</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
         <v>243</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
         <v>244</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
         <v>245</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
         <v>240</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="65" t="s">
         <v>243</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
         <v>244</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
         <v>245</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
         <v>241</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
         <v>242</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
         <v>250</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
         <v>249</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="65" t="s">
         <v>251</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="66" t="s">
         <v>252</v>
       </c>
@@ -2939,14 +2939,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.28515625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="73" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>197</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>198</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>199</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>200</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>201</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>202</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>203</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>25</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>204</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>253</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>205</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>206</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34" t="s">
         <v>207</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>208</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>209</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>210</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>211</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>212</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
         <v>213</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>214</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>215</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>216</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>217</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>219</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>220</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>221</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>222</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>218</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>223</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
         <v>224</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>152</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="34" t="s">
         <v>49</v>
       </c>
@@ -3664,15 +3664,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
         <v>261</v>
       </c>

</xml_diff>

<commit_message>
Added calculation and plotting of winding voltages and flux density, new module for transformer losses, loss and temperature calculation for steady state mode implemented for B2 and B4
</commit_message>
<xml_diff>
--- a/config/magnetics.xlsx
+++ b/config/magnetics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q634145\PycharmProjects\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91CF23F-F82B-4037-8618-D3B85F94CD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82786EFF-61A7-4C42-98E0-84E435976E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="267">
   <si>
     <t>#</t>
   </si>
@@ -746,9 +746,6 @@
   </si>
   <si>
     <t>0127</t>
-  </si>
-  <si>
-    <t>CB</t>
   </si>
   <si>
     <t>sin</t>
@@ -869,7 +866,20 @@
     <t>LD_tra</t>
   </si>
   <si>
+    <t>Transformer Model</t>
+  </si>
+  <si>
+    <t>(con): constant parameters, 
+(tab): tabulated parameters</t>
+  </si>
+  <si>
+    <t>TraMdl</t>
+  </si>
+  <si>
     <t>RL</t>
+  </si>
+  <si>
+    <t>FF</t>
   </si>
 </sst>
 </file>
@@ -1896,7 +1906,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1912,7 +1922,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1944,7 +1954,7 @@
         <v>15</v>
       </c>
       <c r="J13" s="73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K13" s="74"/>
       <c r="L13" s="75"/>
@@ -1969,13 +1979,13 @@
         <v>16</v>
       </c>
       <c r="J14" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="K14" s="46" t="s">
         <v>230</v>
       </c>
-      <c r="K14" s="46" t="s">
+      <c r="L14" s="47" t="s">
         <v>231</v>
-      </c>
-      <c r="L14" s="47" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1999,10 +2009,10 @@
       </c>
       <c r="J15" s="38"/>
       <c r="K15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L15" s="39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2010,13 +2020,13 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" t="s">
         <v>255</v>
-      </c>
-      <c r="C16" t="s">
-        <v>254</v>
-      </c>
-      <c r="D16" t="s">
-        <v>256</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
@@ -2026,10 +2036,10 @@
       </c>
       <c r="J16" s="40"/>
       <c r="K16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L16" s="39" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2038,10 +2048,10 @@
       </c>
       <c r="J17" s="41"/>
       <c r="K17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L17" s="39" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2050,10 +2060,10 @@
       </c>
       <c r="J18" s="42"/>
       <c r="K18" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L18" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2281,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,7 +2444,7 @@
         <v>64</v>
       </c>
       <c r="E8" s="11">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="F8" s="54" t="s">
         <v>4</v>
@@ -2494,7 +2504,7 @@
         <v>66</v>
       </c>
       <c r="E11" s="11">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="F11" s="54" t="s">
         <v>4</v>
@@ -2650,7 +2660,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F2" s="59" t="s">
         <v>22</v>
@@ -2658,7 +2668,7 @@
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="17" t="s">
@@ -2676,7 +2686,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="9" t="s">
@@ -2694,7 +2704,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="9" t="s">
@@ -2712,7 +2722,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="9" t="s">
@@ -2730,7 +2740,7 @@
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="10" t="s">
@@ -2748,7 +2758,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="65" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="9" t="s">
@@ -2766,7 +2776,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="9" t="s">
@@ -2784,7 +2794,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B10" s="48"/>
       <c r="C10" s="9" t="s">
@@ -2802,11 +2812,11 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" s="48"/>
       <c r="C11" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D11" s="51" t="s">
         <v>107</v>
@@ -2820,17 +2830,17 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D12" s="51" t="s">
         <v>108</v>
       </c>
       <c r="E12" s="12">
-        <v>5.0000000000000004E-6</v>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="F12" s="54" t="s">
         <v>118</v>
@@ -2838,11 +2848,11 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D13" s="51" t="s">
         <v>109</v>
@@ -2856,7 +2866,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="9" t="s">
@@ -2874,17 +2884,17 @@
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="65" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D15" s="51" t="s">
         <v>111</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>22</v>
@@ -2892,7 +2902,7 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="66" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B16" s="49"/>
       <c r="C16" s="13" t="s">
@@ -2936,7 +2946,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2974,13 +2984,13 @@
         <v>137</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D2" s="53" t="s">
         <v>35</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="F2" s="56" t="s">
         <v>22</v>
@@ -3148,7 +3158,7 @@
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B11" s="61" t="s">
         <v>137</v>
@@ -3240,7 +3250,7 @@
         <v>35</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F15" s="56" t="s">
         <v>22</v>
@@ -3658,7 +3668,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD1FA08-9341-462A-B6C2-81B791DE91E0}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -3694,26 +3704,47 @@
     </row>
     <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D2" s="70" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="F2" s="72" t="s">
+      <c r="D3" s="51" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="54" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{BBA0E1F0-D60B-4F51-8DC8-2DB1107D8149}">
       <formula1>"NT, OC, SC, RL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3" xr:uid="{F1679C96-EED8-4FF7-9998-EC016E78AC31}">
+      <formula1>"con, tab"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added SysID transformer models and transient operating mode
</commit_message>
<xml_diff>
--- a/config/magnetics.xlsx
+++ b/config/magnetics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q634145\PycharmProjects\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82786EFF-61A7-4C42-98E0-84E435976E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D671465-B4F3-46D3-B44B-5C0DB58B9A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="5" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="270">
   <si>
     <t>#</t>
   </si>
@@ -854,32 +854,42 @@
     <t>B4</t>
   </si>
   <si>
+    <t>Transformer at load side</t>
+  </si>
+  <si>
+    <t>LD_tra</t>
+  </si>
+  <si>
+    <t>Transformer Model</t>
+  </si>
+  <si>
+    <t>(con): constant parameters, 
+(tab): tabulated parameters</t>
+  </si>
+  <si>
+    <t>TraMdl</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
     <t>(NT): no transformer, 
 (OC): open circuit at secondary, 
 (SC): short circuit at secondary, 
-(RL): RL load at secondary</t>
-  </si>
-  <si>
-    <t>Transformer at load side</t>
-  </si>
-  <si>
-    <t>LD_tra</t>
-  </si>
-  <si>
-    <t>Transformer Model</t>
-  </si>
-  <si>
-    <t>(con): constant parameters, 
-(tab): tabulated parameters</t>
-  </si>
-  <si>
-    <t>TraMdl</t>
-  </si>
-  <si>
-    <t>RL</t>
-  </si>
-  <si>
-    <t>FF</t>
+(RL): RL load at secondary, 
+(SS): defined via state space model in para-Excel</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>Plot Downsampling</t>
+  </si>
+  <si>
+    <t>0: no downsampling, 1: downsampling</t>
+  </si>
+  <si>
+    <t>bDS</t>
   </si>
 </sst>
 </file>
@@ -1891,17 +1901,17 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7265625" customWidth="1"/>
+    <col min="5" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +1919,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1917,7 +1927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1925,7 +1935,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1933,8 +1943,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1959,7 +1969,7 @@
       <c r="K13" s="74"/>
       <c r="L13" s="75"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -1988,7 +1998,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -2015,7 +2025,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -2042,7 +2052,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>4</v>
       </c>
@@ -2054,7 +2064,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>5</v>
       </c>
@@ -2080,21 +2090,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CAB857B-5D2E-4BE1-B462-B4B5EEAA4370}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
     <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -2114,7 +2124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
         <v>49</v>
       </c>
@@ -2132,7 +2142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>50</v>
       </c>
@@ -2150,7 +2160,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="34" t="s">
         <v>51</v>
       </c>
@@ -2162,13 +2172,13 @@
         <v>38</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="F4" s="55" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
         <v>52</v>
       </c>
@@ -2180,13 +2190,13 @@
         <v>39</v>
       </c>
       <c r="E5" s="23">
-        <v>10000000</v>
+        <v>1000000000</v>
       </c>
       <c r="F5" s="56" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
         <v>53</v>
       </c>
@@ -2204,7 +2214,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>54</v>
       </c>
@@ -2222,7 +2232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="34" t="s">
         <v>55</v>
       </c>
@@ -2240,8 +2250,26 @@
         <v>22</v>
       </c>
     </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{AC9A4A0E-EBB7-409B-9C1B-00990BA8FA52}">
       <formula1>"0, 1"</formula1>
     </dataValidation>
@@ -2265,7 +2293,11 @@
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5" xr:uid="{E54ED088-4FB7-429D-910B-F71618C430C1}">
       <formula1>10000</formula1>
-      <formula2>1000000000</formula2>
+      <formula2>100000000000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9" xr:uid="{689E22D3-C5CC-472F-842A-9F3F43AFCC7E}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2280,17 +2312,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86190CFD-1D2B-4FE4-A04E-A3C453840C86}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2310,7 +2342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>96</v>
       </c>
@@ -2330,7 +2362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>93</v>
       </c>
@@ -2350,7 +2382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>94</v>
       </c>
@@ -2370,7 +2402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>95</v>
       </c>
@@ -2390,7 +2422,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>85</v>
       </c>
@@ -2404,13 +2436,13 @@
         <v>62</v>
       </c>
       <c r="E6" s="11">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F6" s="54" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>86</v>
       </c>
@@ -2430,7 +2462,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>87</v>
       </c>
@@ -2450,7 +2482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>88</v>
       </c>
@@ -2464,13 +2496,13 @@
         <v>65</v>
       </c>
       <c r="E9" s="11">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="F9" s="54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>89</v>
       </c>
@@ -2484,13 +2516,13 @@
         <v>34</v>
       </c>
       <c r="E10" s="29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>92</v>
       </c>
@@ -2504,13 +2536,13 @@
         <v>66</v>
       </c>
       <c r="E11" s="11">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="F11" s="54" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="27" t="s">
         <v>90</v>
       </c>
@@ -2530,7 +2562,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>91</v>
       </c>
@@ -2544,13 +2576,13 @@
         <v>68</v>
       </c>
       <c r="E13" s="30">
-        <v>0.1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>95</v>
       </c>
@@ -2570,7 +2602,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="27" t="s">
         <v>94</v>
       </c>
@@ -2616,19 +2648,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799FBFCB-8244-4B83-8CC9-EBD2890613E5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2648,7 +2680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="63" t="s">
         <v>126</v>
       </c>
@@ -2666,7 +2698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="64" t="s">
         <v>238</v>
       </c>
@@ -2684,7 +2716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>242</v>
       </c>
@@ -2702,7 +2734,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>243</v>
       </c>
@@ -2720,7 +2752,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="65" t="s">
         <v>244</v>
       </c>
@@ -2738,7 +2770,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="65" t="s">
         <v>239</v>
       </c>
@@ -2756,7 +2788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="65" t="s">
         <v>242</v>
       </c>
@@ -2774,7 +2806,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="65" t="s">
         <v>243</v>
       </c>
@@ -2792,7 +2824,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="65" t="s">
         <v>244</v>
       </c>
@@ -2810,7 +2842,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="65" t="s">
         <v>240</v>
       </c>
@@ -2822,13 +2854,13 @@
         <v>107</v>
       </c>
       <c r="E11" s="12">
-        <v>5.0000000000000001E-4</v>
+        <v>0.05</v>
       </c>
       <c r="F11" s="54" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="65" t="s">
         <v>241</v>
       </c>
@@ -2840,13 +2872,13 @@
         <v>108</v>
       </c>
       <c r="E12" s="12">
-        <v>2.9999999999999999E-7</v>
+        <v>4.9999999999999998E-7</v>
       </c>
       <c r="F12" s="54" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="65" t="s">
         <v>249</v>
       </c>
@@ -2864,7 +2896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="65" t="s">
         <v>248</v>
       </c>
@@ -2882,7 +2914,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="65" t="s">
         <v>250</v>
       </c>
@@ -2900,7 +2932,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="66" t="s">
         <v>251</v>
       </c>
@@ -2945,18 +2977,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.26953125" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2976,7 +3008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="73" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
         <v>197</v>
       </c>
@@ -2990,13 +3022,13 @@
         <v>35</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F2" s="56" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>198</v>
       </c>
@@ -3016,7 +3048,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>199</v>
       </c>
@@ -3036,7 +3068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
         <v>200</v>
       </c>
@@ -3056,7 +3088,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
         <v>201</v>
       </c>
@@ -3076,7 +3108,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>202</v>
       </c>
@@ -3096,7 +3128,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
         <v>203</v>
       </c>
@@ -3116,7 +3148,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
         <v>25</v>
       </c>
@@ -3136,7 +3168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="33" t="s">
         <v>204</v>
       </c>
@@ -3156,7 +3188,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
         <v>252</v>
       </c>
@@ -3176,7 +3208,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="33" t="s">
         <v>205</v>
       </c>
@@ -3190,13 +3222,13 @@
         <v>27</v>
       </c>
       <c r="E12" s="12">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="F12" s="54" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>206</v>
       </c>
@@ -3216,7 +3248,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="34" t="s">
         <v>207</v>
       </c>
@@ -3236,7 +3268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
         <v>208</v>
       </c>
@@ -3256,7 +3288,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="33" t="s">
         <v>209</v>
       </c>
@@ -3276,7 +3308,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="33" t="s">
         <v>210</v>
       </c>
@@ -3296,7 +3328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
         <v>211</v>
       </c>
@@ -3316,7 +3348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="33" t="s">
         <v>212</v>
       </c>
@@ -3336,7 +3368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="33" t="s">
         <v>213</v>
       </c>
@@ -3356,7 +3388,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="34" t="s">
         <v>214</v>
       </c>
@@ -3376,7 +3408,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="32" t="s">
         <v>215</v>
       </c>
@@ -3396,7 +3428,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="33" t="s">
         <v>216</v>
       </c>
@@ -3416,7 +3448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>217</v>
       </c>
@@ -3436,7 +3468,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="33" t="s">
         <v>219</v>
       </c>
@@ -3456,7 +3488,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
         <v>220</v>
       </c>
@@ -3476,7 +3508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="33" t="s">
         <v>221</v>
       </c>
@@ -3496,7 +3528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>222</v>
       </c>
@@ -3516,7 +3548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="33" t="s">
         <v>218</v>
       </c>
@@ -3536,7 +3568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="33" t="s">
         <v>223</v>
       </c>
@@ -3556,7 +3588,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="34" t="s">
         <v>224</v>
       </c>
@@ -3576,7 +3608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
         <v>152</v>
       </c>
@@ -3596,7 +3628,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="34" t="s">
         <v>49</v>
       </c>
@@ -3670,19 +3702,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD1FA08-9341-462A-B6C2-81B791DE91E0}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -3702,34 +3734,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="73" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="67" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D2" s="70" t="s">
+        <v>260</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>266</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
         <v>261</v>
-      </c>
-      <c r="E2" s="71" t="s">
-        <v>265</v>
-      </c>
-      <c r="F2" s="72" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>262</v>
       </c>
       <c r="B3" s="61"/>
       <c r="C3" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="51" t="s">
         <v>263</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>264</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>163</v>
@@ -3741,7 +3773,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{BBA0E1F0-D60B-4F51-8DC8-2DB1107D8149}">
-      <formula1>"NT, OC, SC, RL"</formula1>
+      <formula1>"NT, OC, SC, RL, SS"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3" xr:uid="{F1679C96-EED8-4FF7-9998-EC016E78AC31}">
       <formula1>"con, tab"</formula1>

</xml_diff>